<commit_message>
Add weights for people aged lower than 18
</commit_message>
<xml_diff>
--- a/server/data/backup/Statistik_Menschen.xlsx
+++ b/server/data/backup/Statistik_Menschen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malie\dev\DeMetrics\server\data\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9747350-5122-4866-8E4A-FCB29B65D41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684E45CC-25B4-4A2F-B48F-11BF9E59CDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{5F12B1DA-1378-4AA2-9E22-3E1B15DBE18A}"/>
+    <workbookView xWindow="33660" yWindow="2280" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{5F12B1DA-1378-4AA2-9E22-3E1B15DBE18A}"/>
   </bookViews>
   <sheets>
     <sheet name="Einkommen" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="199">
   <si>
     <t>500.000 € - 1.000.000 €</t>
   </si>
@@ -626,6 +626,21 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>3 - 6</t>
+  </si>
+  <si>
+    <t>7 - 10</t>
+  </si>
+  <si>
+    <t>11 - 13</t>
+  </si>
+  <si>
+    <t>14 - 17</t>
+  </si>
+  <si>
+    <t>Tab 1 in https://www.rki.de/DE/Content/Kommissionen/Bundesgesundheitsblatt/Downloads/2019_10_Schienkiewitz_BMI.pdf?__blob=publicationFile</t>
   </si>
 </sst>
 </file>
@@ -634,7 +649,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="196" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -693,7 +708,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -713,7 +728,8 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="196" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1256,7 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1445DA-59FA-49FC-963C-D26736079AAA}">
   <dimension ref="A1:CV104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
@@ -4390,10 +4406,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77458E25-B2BB-45B6-851B-F4AA4B31A698}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4404,555 +4420,752 @@
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="C2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="C4" t="s">
         <v>154</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>164</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E4" t="s">
         <v>165</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>185</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>186</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>187</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D5" t="s">
         <v>188</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" t="s">
         <v>189</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F5" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4">
-        <v>1.2</v>
-      </c>
-      <c r="D4">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="E4">
-        <v>41.6</v>
-      </c>
-      <c r="F4">
-        <v>19.100000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C5">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D5">
-        <v>65.099999999999994</v>
-      </c>
-      <c r="E5">
-        <v>25</v>
-      </c>
-      <c r="F5">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>158</v>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>194</v>
       </c>
       <c r="B6" t="s">
         <v>191</v>
       </c>
       <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>86.7</v>
+      </c>
+      <c r="E6">
+        <v>6.4</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>48.8</v>
-      </c>
-      <c r="E6">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="F6">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>159</v>
+      <c r="G6">
+        <f>SUM(C6:F6)</f>
+        <v>100.10000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>195</v>
       </c>
       <c r="B7" t="s">
         <v>191</v>
       </c>
       <c r="C7">
-        <v>0.9</v>
+        <v>7.6</v>
       </c>
       <c r="D7">
-        <v>38.9</v>
+        <v>76.3</v>
       </c>
       <c r="E7">
-        <v>40.1</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="F7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>160</v>
+        <v>6.8</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G9" si="0">SUM(C7:F7)</f>
+        <v>99.999999999999986</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>196</v>
       </c>
       <c r="B8" t="s">
         <v>191</v>
       </c>
       <c r="C8">
-        <v>0.7</v>
+        <v>8.5</v>
       </c>
       <c r="D8">
-        <v>30.8</v>
+        <v>70.400000000000006</v>
       </c>
       <c r="E8">
-        <v>45.1</v>
+        <v>13.1</v>
       </c>
       <c r="F8">
-        <v>23.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>161</v>
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="B9" t="s">
         <v>191</v>
       </c>
       <c r="C9">
-        <v>1.3</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D9">
-        <v>30</v>
+        <v>71.7</v>
       </c>
       <c r="E9">
-        <v>45.1</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="F9">
-        <v>23.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>162</v>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>99.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>156</v>
       </c>
       <c r="B10" t="s">
         <v>191</v>
       </c>
       <c r="C10">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
       <c r="D10">
-        <v>26.7</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="E10">
-        <v>48.4</v>
+        <v>41.6</v>
       </c>
       <c r="F10">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
         <v>191</v>
       </c>
       <c r="C11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D11">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="E11">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>48.8</v>
+      </c>
+      <c r="E12">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="F12">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13">
+        <v>0.9</v>
+      </c>
+      <c r="D13">
+        <v>38.9</v>
+      </c>
+      <c r="E13">
+        <v>40.1</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14">
+        <v>0.7</v>
+      </c>
+      <c r="D14">
+        <v>30.8</v>
+      </c>
+      <c r="E14">
+        <v>45.1</v>
+      </c>
+      <c r="F14">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C15">
+        <v>1.3</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+      <c r="E15">
+        <v>45.1</v>
+      </c>
+      <c r="F15">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C16">
+        <v>0.4</v>
+      </c>
+      <c r="D16">
+        <v>26.7</v>
+      </c>
+      <c r="E16">
+        <v>48.4</v>
+      </c>
+      <c r="F16">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17">
         <v>0.6</v>
       </c>
-      <c r="D11">
+      <c r="D17">
         <v>36.299999999999997</v>
       </c>
-      <c r="E11">
+      <c r="E17">
         <v>48.8</v>
       </c>
-      <c r="F11">
+      <c r="F17">
         <v>14.3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="18" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18">
+        <v>4.3</v>
+      </c>
+      <c r="D18">
+        <v>84.8</v>
+      </c>
+      <c r="E18">
+        <v>7.6</v>
+      </c>
+      <c r="F18">
+        <v>3.2</v>
+      </c>
+      <c r="G18">
+        <f>SUM(C18:F18)</f>
+        <v>99.899999999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C19">
+        <v>9.6</v>
+      </c>
+      <c r="D19">
+        <v>75.5</v>
+      </c>
+      <c r="E19">
+        <v>10.3</v>
+      </c>
+      <c r="F19">
+        <v>4.7</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ref="G19:G21" si="1">SUM(C19:F19)</f>
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20">
+        <v>7.7</v>
+      </c>
+      <c r="D20">
+        <v>72.3</v>
+      </c>
+      <c r="E20">
+        <v>13.5</v>
+      </c>
+      <c r="F20">
+        <v>6.5</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21">
+        <v>7.3</v>
+      </c>
+      <c r="D21">
+        <v>76.5</v>
+      </c>
+      <c r="E21">
+        <v>8.5</v>
+      </c>
+      <c r="F21">
+        <v>7.7</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>156</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B22" t="s">
         <v>192</v>
       </c>
-      <c r="C12">
+      <c r="C22">
         <v>3.4</v>
       </c>
-      <c r="D12">
+      <c r="D22">
         <v>50</v>
       </c>
-      <c r="E12">
+      <c r="E22">
         <v>27.5</v>
       </c>
-      <c r="F12">
+      <c r="F22">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>157</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B23" t="s">
         <v>192</v>
       </c>
-      <c r="C13">
+      <c r="C23">
         <v>7.6</v>
       </c>
-      <c r="D13">
+      <c r="D23">
         <v>66.7</v>
       </c>
-      <c r="E13">
+      <c r="E23">
         <v>15.7</v>
       </c>
-      <c r="F13">
+      <c r="F23">
         <v>9.9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>158</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B24" t="s">
         <v>192</v>
       </c>
-      <c r="C14">
+      <c r="C24">
         <v>7.3</v>
       </c>
-      <c r="D14">
+      <c r="D24">
         <v>62.1</v>
       </c>
-      <c r="E14">
+      <c r="E24">
         <v>19.899999999999999</v>
       </c>
-      <c r="F14">
+      <c r="F24">
         <v>10.7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>159</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B25" t="s">
         <v>192</v>
       </c>
-      <c r="C15">
+      <c r="C25">
         <v>2.5</v>
       </c>
-      <c r="D15">
+      <c r="D25">
         <v>53.4</v>
       </c>
-      <c r="E15">
+      <c r="E25">
         <v>28.1</v>
       </c>
-      <c r="F15">
+      <c r="F25">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>160</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B26" t="s">
         <v>192</v>
       </c>
-      <c r="C16">
+      <c r="C26">
         <v>1.9</v>
       </c>
-      <c r="D16">
+      <c r="D26">
         <v>51.9</v>
       </c>
-      <c r="E16">
+      <c r="E26">
         <v>26.6</v>
       </c>
-      <c r="F16">
+      <c r="F26">
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>161</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B27" t="s">
         <v>192</v>
       </c>
-      <c r="C17">
+      <c r="C27">
         <v>2.1</v>
       </c>
-      <c r="D17">
+      <c r="D27">
         <v>42</v>
       </c>
-      <c r="E17">
+      <c r="E27">
         <v>29.4</v>
       </c>
-      <c r="F17">
+      <c r="F27">
         <v>26.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>162</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B28" t="s">
         <v>192</v>
       </c>
-      <c r="C18">
+      <c r="C28">
         <v>1.4</v>
       </c>
-      <c r="D18">
+      <c r="D28">
         <v>38.6</v>
       </c>
-      <c r="E18">
+      <c r="E28">
         <v>33.6</v>
       </c>
-      <c r="F18">
+      <c r="F28">
         <v>26.4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>163</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B29" t="s">
         <v>192</v>
       </c>
-      <c r="C19">
+      <c r="C29">
         <v>3.4</v>
       </c>
-      <c r="D19">
+      <c r="D29">
         <v>43.3</v>
       </c>
-      <c r="E19">
+      <c r="E29">
         <v>34.1</v>
       </c>
-      <c r="F19">
+      <c r="F29">
         <v>19.3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>156</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B30" t="s">
         <v>193</v>
       </c>
-      <c r="C20">
-        <f t="shared" ref="C20:F27" si="0">(C4+C12)/2</f>
+      <c r="C30">
+        <f t="shared" ref="C30:F37" si="2">(C10+C22)/2</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
+      <c r="D30">
+        <f t="shared" si="2"/>
         <v>44.1</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
+      <c r="E30">
+        <f t="shared" si="2"/>
         <v>34.549999999999997</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
+      <c r="F30">
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>157</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B31" t="s">
         <v>193</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
+      <c r="C31">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
+      <c r="D31">
+        <f t="shared" si="2"/>
         <v>65.900000000000006</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
+      <c r="E31">
+        <f t="shared" si="2"/>
         <v>20.350000000000001</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
+      <c r="F31">
+        <f t="shared" si="2"/>
         <v>7.75</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>158</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B32" t="s">
         <v>193</v>
       </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
+      <c r="C32">
+        <f t="shared" si="2"/>
         <v>4.1500000000000004</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
+      <c r="D32">
+        <f t="shared" si="2"/>
         <v>55.45</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
+      <c r="E32">
+        <f t="shared" si="2"/>
         <v>27.349999999999998</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
+      <c r="F32">
+        <f t="shared" si="2"/>
         <v>13.05</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>159</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B33" t="s">
         <v>193</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
+      <c r="C33">
+        <f t="shared" si="2"/>
         <v>1.7</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
+      <c r="D33">
+        <f t="shared" si="2"/>
         <v>46.15</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
+      <c r="E33">
+        <f t="shared" si="2"/>
         <v>34.1</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
+      <c r="F33">
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>160</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B34" t="s">
         <v>193</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
+      <c r="C34">
+        <f t="shared" si="2"/>
         <v>1.2999999999999998</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
+      <c r="D34">
+        <f t="shared" si="2"/>
         <v>41.35</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
+      <c r="E34">
+        <f t="shared" si="2"/>
         <v>35.85</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
+      <c r="F34">
+        <f t="shared" si="2"/>
         <v>21.5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>161</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B35" t="s">
         <v>193</v>
       </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
+      <c r="C35">
+        <f t="shared" si="2"/>
         <v>1.7000000000000002</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
+      <c r="D35">
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
+      <c r="E35">
+        <f t="shared" si="2"/>
         <v>37.25</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
+      <c r="F35">
+        <f t="shared" si="2"/>
         <v>25.1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>162</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B36" t="s">
         <v>193</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
+      <c r="C36">
+        <f t="shared" si="2"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
+      <c r="D36">
+        <f t="shared" si="2"/>
         <v>32.65</v>
       </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
+      <c r="E36">
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
+      <c r="F36">
+        <f t="shared" si="2"/>
         <v>25.45</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>163</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B37" t="s">
         <v>193</v>
       </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
+      <c r="C37">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
+      <c r="D37">
+        <f t="shared" si="2"/>
         <v>39.799999999999997</v>
       </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
+      <c r="E37">
+        <f t="shared" si="2"/>
         <v>41.45</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
+      <c r="F37">
+        <f t="shared" si="2"/>
         <v>16.8</v>
       </c>
     </row>

</xml_diff>